<commit_message>
Update included example data
</commit_message>
<xml_diff>
--- a/Example/Parts List.xlsx
+++ b/Example/Parts List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Programming\BOM program\python-BOM\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C012B935-5A1A-40B3-BA81-EEFAEC84A984}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B152639F-0C9E-469C-8AB9-D735879A6A7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17460" yWindow="5730" windowWidth="15105" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="3375" windowWidth="15105" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
   <si>
     <t>Description</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>McMaster-Carr</t>
-  </si>
-  <si>
     <t>Pkg Price</t>
   </si>
   <si>
@@ -57,12 +54,6 @@
     <t>1/4-20 Hex nut</t>
   </si>
   <si>
-    <t>92220A186</t>
-  </si>
-  <si>
-    <t>95479A111</t>
-  </si>
-  <si>
     <t>PN</t>
   </si>
   <si>
@@ -78,37 +69,85 @@
     <t>Bearing</t>
   </si>
   <si>
-    <t>Axle screw</t>
-  </si>
-  <si>
-    <t>Wheel Nut</t>
-  </si>
-  <si>
-    <t>198457-01</t>
-  </si>
-  <si>
-    <t>198458-01</t>
-  </si>
-  <si>
-    <t>198459-01</t>
-  </si>
-  <si>
-    <t>198460-01</t>
-  </si>
-  <si>
-    <t>198461-01</t>
-  </si>
-  <si>
-    <t>198462-01</t>
-  </si>
-  <si>
-    <t>198463-01</t>
-  </si>
-  <si>
-    <t>Truck</t>
-  </si>
-  <si>
     <t>Truck screw</t>
+  </si>
+  <si>
+    <t>Truck half</t>
+  </si>
+  <si>
+    <t>XYZ Bearing Co.</t>
+  </si>
+  <si>
+    <t>Bolts R Us</t>
+  </si>
+  <si>
+    <t>Skatr Dude Inc.</t>
+  </si>
+  <si>
+    <t>Wheel bearing</t>
+  </si>
+  <si>
+    <t>Truck fixed</t>
+  </si>
+  <si>
+    <t>Truck movable</t>
+  </si>
+  <si>
+    <t>Hard clear urethane</t>
+  </si>
+  <si>
+    <t>Standard type</t>
+  </si>
+  <si>
+    <t>BRX-02</t>
+  </si>
+  <si>
+    <t>TR1-B</t>
+  </si>
+  <si>
+    <t>TR1-A</t>
+  </si>
+  <si>
+    <t>WHL-PRX</t>
+  </si>
+  <si>
+    <t>74295-942</t>
+  </si>
+  <si>
+    <t>92220A</t>
+  </si>
+  <si>
+    <t>95479A</t>
+  </si>
+  <si>
+    <t>SK1001-01</t>
+  </si>
+  <si>
+    <t>SK1002-01</t>
+  </si>
+  <si>
+    <t>SK1007-01</t>
+  </si>
+  <si>
+    <t>SK1006-01</t>
+  </si>
+  <si>
+    <t>SK1005-01</t>
+  </si>
+  <si>
+    <t>SK1004-01</t>
+  </si>
+  <si>
+    <t>SK1003-01</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>part</t>
+  </si>
+  <si>
+    <t>Nut</t>
   </si>
 </sst>
 </file>
@@ -193,7 +232,48 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -204,6 +284,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{867782B6-D9F8-440B-9D21-61C6AF3CEC31}" name="Table1" displayName="Table1" ref="A1:H8" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:H8" xr:uid="{16DF1165-1727-43E0-9852-15718F25DD46}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G8">
+    <sortCondition ref="B1:B8"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{4A460654-0A0D-403D-879D-BCF45C2DE9AF}" name="PN" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{CB1849EF-1C55-4A3A-A614-1FC32B3B636D}" name="Name" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DFD40929-53BD-40B7-93FA-087C02ED4333}" name="Description"/>
+    <tableColumn id="4" xr3:uid="{0F36D6F5-EECE-4979-A3D2-06182AD7BE6D}" name="Supplier" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{41B7A312-6196-4F27-A1F5-835C913CEF83}" name="Supplier PN" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{E30BE2B9-4D32-47C6-BE03-E27FC3346B9F}" name="Pkg QTY"/>
+    <tableColumn id="7" xr3:uid="{D2433C6A-4B68-446D-9B51-36A3F60836F3}" name="Pkg Price" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{4133C43D-AC91-41B3-B974-066EC9093120}" name="Item" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -469,26 +569,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G62"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>2</v>
@@ -500,122 +600,201 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.99</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>15.99</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="1">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>12.25</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="1">
+        <v>50</v>
+      </c>
+      <c r="G6" s="1">
+        <v>12.86</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="6">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="G7" s="1">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1">
         <v>50</v>
       </c>
-      <c r="G2" s="1">
-        <v>12.86</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1">
-        <v>50</v>
-      </c>
-      <c r="G3" s="1">
+      <c r="G8" s="1">
         <v>4.88</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="1"/>
@@ -623,7 +802,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="1"/>
@@ -631,15 +810,16 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -648,34 +828,34 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="5"/>
+      <c r="F15" s="1"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -693,7 +873,6 @@
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -701,7 +880,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="B19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -709,7 +888,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="3"/>
+      <c r="B20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -726,6 +905,7 @@
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -759,16 +939,16 @@
       <c r="G25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
@@ -784,9 +964,7 @@
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
@@ -794,6 +972,7 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
     </row>
@@ -816,6 +995,7 @@
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -824,7 +1004,6 @@
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -833,6 +1012,7 @@
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -859,7 +1039,6 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -869,7 +1048,6 @@
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
     </row>
@@ -877,6 +1055,7 @@
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
     </row>
@@ -891,6 +1070,7 @@
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -898,8 +1078,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="B43" s="4"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -907,7 +1086,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="4"/>
+      <c r="B44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -916,6 +1095,7 @@
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -924,7 +1104,6 @@
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -933,6 +1112,7 @@
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -944,16 +1124,15 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="5"/>
+      <c r="F49" s="1"/>
       <c r="G49" s="1"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1052,17 +1231,12 @@
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>